<commit_message>
add secondary phone to dairy farm producer report
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Farm_Producers_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Farm_Producers_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C167C4D-4F8A-4544-9AD2-95DDA80A9E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D890BF-BA3E-4ED6-80F9-741A157D024F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7EA0AD6D-E727-49F3-939D-8C438C011AC1}"/>
+    <workbookView xWindow="41055" yWindow="4680" windowWidth="28470" windowHeight="10395" xr2:uid="{7EA0AD6D-E727-49F3-939D-8C438C011AC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Producer Contacts</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>{d.Reg[i].PrincipalPhone2}</t>
+  </si>
+  <si>
+    <t>Secondary Phone Number</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].SiteContactPhone2}</t>
   </si>
 </sst>
 </file>
@@ -145,16 +154,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,26 +503,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A396B4-7136-4033-A3E0-61DDCE5F750E}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="5" max="6" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -518,7 +532,7 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E1" t="s">
@@ -531,68 +545,74 @@
         <v>8</v>
       </c>
       <c r="H1" s="4"/>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -609,19 +629,25 @@
         <v>16</v>
       </c>
       <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>

</xml_diff>